<commit_message>
revised sop, elif bugfix, invalid flow term exception
</commit_message>
<xml_diff>
--- a/output/cpc-bile-salt.xlsx
+++ b/output/cpc-bile-salt.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatho\Dropbox\Code\Python\docx-sop-parser\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5036F98C-32C4-4F96-99E2-0289581C3289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
   <si>
-    <t>STEP NUMBER</t>
+    <t>LINE NUMBER</t>
   </si>
   <si>
     <t>KEY</t>
@@ -205,8 +199,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,14 +237,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -297,7 +283,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -329,27 +315,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -381,24 +349,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -574,19 +524,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="39.54296875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -597,7 +542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -608,7 +553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -619,7 +564,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -630,7 +575,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -641,7 +586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -652,7 +597,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -663,7 +608,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -674,7 +619,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -685,7 +630,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -696,7 +641,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -707,7 +652,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>7</v>
       </c>
@@ -718,7 +663,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>7</v>
       </c>
@@ -729,7 +674,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -740,7 +685,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -751,7 +696,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>9</v>
       </c>
@@ -762,7 +707,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>9</v>
       </c>
@@ -773,7 +718,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>10</v>
       </c>
@@ -784,7 +729,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>10</v>
       </c>
@@ -795,7 +740,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>11</v>
       </c>
@@ -806,7 +751,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>12</v>
       </c>
@@ -817,7 +762,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>12</v>
       </c>
@@ -828,7 +773,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>13</v>
       </c>
@@ -839,7 +784,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>13</v>
       </c>
@@ -850,7 +795,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>14</v>
       </c>
@@ -861,7 +806,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>16</v>
       </c>
@@ -872,7 +817,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>16</v>
       </c>
@@ -883,7 +828,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>17</v>
       </c>
@@ -894,7 +839,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -905,7 +850,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>19</v>
       </c>
@@ -916,7 +861,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>19</v>
       </c>
@@ -927,7 +872,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>19</v>
       </c>
@@ -938,7 +883,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>19</v>
       </c>
@@ -949,7 +894,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>19</v>
       </c>
@@ -960,7 +905,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>20</v>
       </c>
@@ -971,7 +916,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>20</v>
       </c>
@@ -982,7 +927,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>20</v>
       </c>
@@ -993,7 +938,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>20</v>
       </c>
@@ -1004,7 +949,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>21</v>
       </c>
@@ -1015,7 +960,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>21</v>
       </c>
@@ -1026,7 +971,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>21</v>
       </c>
@@ -1037,7 +982,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3">
       <c r="A42">
         <v>22</v>
       </c>
@@ -1048,7 +993,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3">
       <c r="A43">
         <v>22</v>
       </c>
@@ -1059,7 +1004,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3">
       <c r="A44">
         <v>22</v>
       </c>
@@ -1070,7 +1015,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3">
       <c r="A45">
         <v>23</v>
       </c>
@@ -1081,7 +1026,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3">
       <c r="A46">
         <v>23</v>
       </c>
@@ -1092,7 +1037,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -1103,7 +1048,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3">
       <c r="A48">
         <v>25</v>
       </c>
@@ -1114,7 +1059,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3">
       <c r="A49">
         <v>25</v>
       </c>
@@ -1125,7 +1070,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3">
       <c r="A50">
         <v>25</v>
       </c>
@@ -1136,7 +1081,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3">
       <c r="A51">
         <v>25</v>
       </c>
@@ -1147,7 +1092,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3">
       <c r="A52">
         <v>26</v>
       </c>
@@ -1158,7 +1103,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
rearrange sample.py into tidied up function
</commit_message>
<xml_diff>
--- a/output/cpc-bile-salt.xlsx
+++ b/output/cpc-bile-salt.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
   <si>
-    <t>LINE NUMBER</t>
+    <t>PARAGRAPH NUMBER</t>
   </si>
   <si>
     <t>KEY</t>
@@ -555,7 +555,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -577,7 +577,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -610,7 +610,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -621,7 +621,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
@@ -654,7 +654,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
@@ -698,7 +698,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>30</v>
@@ -709,7 +709,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
         <v>32</v>
@@ -720,7 +720,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>34</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
         <v>36</v>
@@ -742,7 +742,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
         <v>38</v>
@@ -753,7 +753,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
         <v>40</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
         <v>32</v>
@@ -775,7 +775,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
         <v>34</v>
@@ -786,7 +786,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
         <v>36</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B25" t="s">
         <v>38</v>
@@ -808,7 +808,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
         <v>34</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
         <v>36</v>
@@ -830,7 +830,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
         <v>38</v>
@@ -852,7 +852,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
         <v>45</v>
@@ -863,7 +863,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
         <v>47</v>
@@ -874,7 +874,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
         <v>32</v>
@@ -885,7 +885,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
         <v>48</v>
@@ -896,7 +896,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
         <v>18</v>
@@ -907,7 +907,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
         <v>47</v>
@@ -918,7 +918,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
         <v>45</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
         <v>18</v>
@@ -940,7 +940,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
         <v>48</v>
@@ -951,7 +951,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B39" t="s">
         <v>47</v>
@@ -962,7 +962,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
         <v>45</v>
@@ -973,7 +973,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
         <v>32</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
         <v>47</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
         <v>45</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B44" t="s">
         <v>45</v>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B45" t="s">
         <v>47</v>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
         <v>32</v>
@@ -1050,7 +1050,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
         <v>45</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B50" t="s">
         <v>54</v>
@@ -1083,7 +1083,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B51" t="s">
         <v>56</v>
@@ -1094,7 +1094,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B52" t="s">
         <v>58</v>

</xml_diff>